<commit_message>
step by step till success
</commit_message>
<xml_diff>
--- a/工作文档/加班统计/赵行保加班调休统计.xlsx
+++ b/工作文档/加班统计/赵行保加班调休统计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12600" activeTab="4"/>
+    <workbookView windowWidth="21600" windowHeight="8370" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="三月加班调休统计" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="五月加班调休统计" sheetId="3" r:id="rId3"/>
     <sheet name="六月加班调休统计" sheetId="4" r:id="rId4"/>
     <sheet name="七月加班调休" sheetId="5" r:id="rId5"/>
+    <sheet name="八月加班调休" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="44">
   <si>
     <t>加班</t>
   </si>
@@ -143,10 +144,13 @@
     <t>19:00-21:06</t>
   </si>
   <si>
-    <t>9:00-10:00</t>
+    <t>9:00-11:00</t>
   </si>
   <si>
     <t>19:00-20:40</t>
+  </si>
+  <si>
+    <t>19:00-00:30</t>
   </si>
 </sst>
 </file>
@@ -154,12 +158,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,8 +193,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -204,25 +209,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,6 +235,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -252,22 +257,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,16 +271,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,16 +294,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,6 +349,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -364,43 +373,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,25 +505,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,91 +517,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,6 +602,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -625,6 +631,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -636,26 +668,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -674,160 +686,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2404,8 +2401,8 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -2503,7 +2500,7 @@
         <v>41</v>
       </c>
       <c r="F5" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2537,7 +2534,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2643,7 +2640,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="15">
         <f>SUM(F3:F18)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2656,7 +2653,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3">
         <f>C19-F19</f>
-        <v>-14</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2669,7 +2666,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="3">
         <f>55+F20</f>
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2685,4 +2682,251 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="12.25" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4">
+        <v>43678</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43679</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8">
+        <f>SUM(C3:C18)</f>
+        <v>5.5</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15">
+        <f>SUM(F3:F18)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="3">
+        <f>C19-F19</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="3">
+        <f>39+F20</f>
+        <v>41.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:E21"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>